<commit_message>
Added notes to models.xlsx to point formatting reccomendations; Added colorized text to console for a more easy reading; Fixed bugs on filling channels_dict and optimized search for header indexes; added more steps to automation to avoid mistakes; enshorted timings for clicks and key presses
</commit_message>
<xml_diff>
--- a/model.xlsx
+++ b/model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\Personal Projects\AddUsersToSlackChannelsAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E62798-A5DA-42B7-9D51-5928D5D68692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04ECC8C6-0833-4B14-B597-D447FF6E1E0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7039" yWindow="4266" windowWidth="27467" windowHeight="14185" xr2:uid="{49CC6859-8533-3845-9891-DE68C4BE53FE}"/>
+    <workbookView xWindow="1710" yWindow="900" windowWidth="19530" windowHeight="15300" xr2:uid="{49CC6859-8533-3845-9891-DE68C4BE53FE}"/>
   </bookViews>
   <sheets>
     <sheet name="slack" sheetId="1" r:id="rId1"/>
@@ -35,6 +35,66 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Marcelo</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{F18619C2-E7A3-48DF-AA2C-0876193646F5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Marcelo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Make sure to:
+select this entire column and format it as text fields;
+remove ALL hyperlinks after inserting e-mails</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{340CCABA-2EAB-4B6C-B187-247927C4053D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Marcelo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Make sure to select this entire column and format it as Text Fields</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
   <si>
@@ -114,7 +174,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -142,6 +202,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -185,6 +258,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -497,17 +574,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC5AE89-BF2A-1E48-9CED-1A56375A9BAE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC5AE89-BF2A-1E48-9CED-1A56375A9BAE}">
   <dimension ref="A1:B516"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.08984375" customWidth="1"/>
+    <col min="1" max="1" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.08203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -693,8 +770,9 @@
     <hyperlink ref="A3:A21" r:id="rId2" display="user@email.com" xr:uid="{806A2FF1-DAB4-41C9-9781-762DC8247301}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>